<commit_message>
Update sample file for highlight duplicate items
</commit_message>
<xml_diff>
--- a/resources/sample/booth_import_sample.xlsx
+++ b/resources/sample/booth_import_sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -134,7 +134,18 @@
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="合計" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -443,12 +454,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -504,6 +515,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add zone in Booth
</commit_message>
<xml_diff>
--- a/resources/sample/booth_import_sample.xlsx
+++ b/resources/sample/booth_import_sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CheckIn2017\resources\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CheckIn\resources\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA49F88-9925-40AC-A765-BFD2CE7117D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>攤位編號</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -48,6 +49,17 @@
   <si>
     <t>門口01</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>分區</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>甲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>乙</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,27 @@
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="合計" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -455,68 +487,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>24.179244000000001</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>120.648332</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>24.179416</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>120.648353</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>24.178820000000002</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>120.64666200000001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>